<commit_message>
Change Vietnam to Viet Nam
</commit_message>
<xml_diff>
--- a/InputData/OGHIST.xlsx
+++ b/InputData/OGHIST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/hmaeda_worldbank_org/Documents/CodeMaps/Country/FY24/Final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB514665\OneDrive - WBG\PovcalNet\GitHub\Class\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{5DD3E766-65A0-47BB-B916-ECAFA47A0AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37A38C20-7EC7-43D6-8C3C-5F94C425B13D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5120DC-8D6A-4284-B07C-8E1795356CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="730" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9270" yWindow="3390" windowWidth="15900" windowHeight="11175" tabRatio="730" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="5" state="hidden" r:id="rId1"/>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14746" uniqueCount="944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14746" uniqueCount="945">
   <si>
     <t>Document:</t>
   </si>
@@ -3059,6 +3059,9 @@
   </si>
   <si>
     <t>4,466 - 13,845</t>
+  </si>
+  <si>
+    <t>Viet Nam</t>
   </si>
 </sst>
 </file>
@@ -4482,7 +4485,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Parameters"/>
@@ -4600,9 +4603,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4640,9 +4643,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4675,26 +4678,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4727,26 +4713,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5027,7 +4996,7 @@
   </sheetPr>
   <dimension ref="A1:AY47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="AU8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
@@ -7157,11 +7126,11 @@
   </sheetPr>
   <dimension ref="A1:IU240"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="2" ySplit="10" topLeftCell="AG29" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane xSplit="2" ySplit="10" topLeftCell="AG211" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="AP32" sqref="AP32"/>
+      <selection pane="bottomRight" activeCell="B225" sqref="B225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -32712,7 +32681,7 @@
         <v>540</v>
       </c>
       <c r="B224" s="66" t="s">
-        <v>541</v>
+        <v>944</v>
       </c>
       <c r="C224" s="6" t="s">
         <v>548</v>
@@ -55247,33 +55216,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <i008215bacac45029ee8cafff4c8e93b xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DECDG - Development Data Group</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">2ae5ce6c-bf4c-4936-8a28-da4d57c09588</TermId>
-        </TermInfo>
-      </Terms>
-    </i008215bacac45029ee8cafff4c8e93b>
-    <Abstract xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <WBDocs_Access_To_Info_Exception xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">12. Not Assessed</WBDocs_Access_To_Info_Exception>
-    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Value>-1</Value>
-    </TaxCatchAll>
-    <o1cb080a3dca4eb8a0fd03c7cc8bf8f7 xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </o1cb080a3dca4eb8a0fd03c7cc8bf8f7>
-    <OneCMS_Subcategory xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <WBDocs_Information_Classification xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">Official Use Only</WBDocs_Information_Classification>
-    <OneCMS_Category xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <WBDocs_Document_Date xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">2023-06-26T15:05:53+00:00</WBDocs_Document_Date>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2a6c10d7-b926-4fc0-945e-3cbf5049f6bd" ContentTypeId="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F02" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="WBDocument" ma:contentTypeID="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F0200DC389410BEDF94408689F8CB0B5B3F0C" ma:contentTypeVersion="29" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="eb8de44df1138b2c143719e7030b0535">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e02667f-0271-471b-bd6e-11a2e16def1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c21bbd07aabf60030dcf23967a052890" ns3:_="">
     <xsd:import namespace="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
@@ -55515,14 +55467,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2a6c10d7-b926-4fc0-945e-3cbf5049f6bd" ContentTypeId="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F02" PreviousValue="false"/>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <i008215bacac45029ee8cafff4c8e93b xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DECDG - Development Data Group</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">2ae5ce6c-bf4c-4936-8a28-da4d57c09588</TermId>
+        </TermInfo>
+      </Terms>
+    </i008215bacac45029ee8cafff4c8e93b>
+    <Abstract xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <WBDocs_Access_To_Info_Exception xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">12. Not Assessed</WBDocs_Access_To_Info_Exception>
+    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Value>-1</Value>
+    </TaxCatchAll>
+    <o1cb080a3dca4eb8a0fd03c7cc8bf8f7 xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </o1cb080a3dca4eb8a0fd03c7cc8bf8f7>
+    <OneCMS_Subcategory xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <WBDocs_Information_Classification xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">Official Use Only</WBDocs_Information_Classification>
+    <OneCMS_Category xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <WBDocs_Document_Date xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">2023-06-26T15:05:53+00:00</WBDocs_Document_Date>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55535,16 +55504,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CA08370-99A5-4FA5-A2C3-E68D6DF39C51}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DB51E32-A88A-4A12-90DD-F41DD2BB57BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E0163D1-75F3-479B-97C7-B5428585AAD7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BABE3842-BECA-4BDF-B0D9-43E38B539FED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -55562,18 +55537,12 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E0163D1-75F3-479B-97C7-B5428585AAD7}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CA08370-99A5-4FA5-A2C3-E68D6DF39C51}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DB51E32-A88A-4A12-90DD-F41DD2BB57BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>